<commit_message>
Integrated new experiments into manuscript.
</commit_message>
<xml_diff>
--- a/python/event_results/results.xlsx
+++ b/python/event_results/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <sheet name="CC005" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="CC026" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="CC090" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Obscuring Profile" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="40">
   <si>
     <t xml:space="preserve">test_x</t>
   </si>
@@ -116,6 +117,39 @@
   </si>
   <si>
     <t xml:space="preserve">CC090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison of Line Segments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stderr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diff dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t stat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p</t>
   </si>
 </sst>
 </file>
@@ -127,7 +161,7 @@
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,12 +191,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <i val="true"/>
@@ -349,19 +377,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,111 +405,111 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,17 +532,17 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,7 +602,7 @@
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">AVERAGE(CC011:CC090!B3:B3)</f>
-        <v>0.999828802214728</v>
+        <v>0.999828802214729</v>
       </c>
       <c r="C4" s="8" t="n">
         <f aca="false">AVERAGE(CC011:CC090!C3:C3)</f>
@@ -636,29 +664,29 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15" t="n">
+      <c r="B7" s="14" t="n">
         <f aca="false">SUM(CC011:CC090!B6:B6)</f>
         <v>9</v>
       </c>
-      <c r="C7" s="16" t="n">
+      <c r="C7" s="10" t="n">
         <f aca="false">SUM(CC011:CC090!C6:C6)</f>
         <v>5</v>
       </c>
-      <c r="D7" s="17" t="n">
+      <c r="D7" s="15" t="n">
         <f aca="false">SUM(CC011:CC090!D6:D6)</f>
         <v>6</v>
       </c>
@@ -692,15 +720,15 @@
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15" t="n">
+      <c r="B8" s="14" t="n">
         <f aca="false">SUM(CC011:CC090!B7:B7)</f>
         <v>9</v>
       </c>
-      <c r="C8" s="16" t="n">
+      <c r="C8" s="10" t="n">
         <f aca="false">SUM(CC011:CC090!C7:C7)</f>
         <v>6</v>
       </c>
-      <c r="D8" s="17" t="n">
+      <c r="D8" s="15" t="n">
         <f aca="false">SUM(CC011:CC090!D7:D7)</f>
         <v>5</v>
       </c>
@@ -710,58 +738,58 @@
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="15" t="n">
+      <c r="B9" s="14" t="n">
         <f aca="false">SUM(CC011:CC090!B8:B8)</f>
         <v>8</v>
       </c>
-      <c r="C9" s="16" t="n">
+      <c r="C9" s="10" t="n">
         <f aca="false">SUM(CC011:CC090!C8:C8)</f>
         <v>4</v>
       </c>
-      <c r="D9" s="17" t="n">
+      <c r="D9" s="15" t="n">
         <f aca="false">SUM(CC011:CC090!D8:D8)</f>
         <v>7</v>
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
+    <row r="10" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24" t="n">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22" t="n">
         <f aca="false">SUM(C7:C9)</f>
         <v>15</v>
       </c>
-      <c r="D11" s="24" t="n">
+      <c r="D11" s="22" t="n">
         <f aca="false">SUM(D7:D9)</f>
         <v>18</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25" t="s">
+      <c r="E11" s="22"/>
+      <c r="F11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27" t="n">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25" t="n">
         <f aca="false">SUM(B7:B9)-C11</f>
         <v>11</v>
       </c>
-      <c r="D12" s="27" t="n">
+      <c r="D12" s="25" t="n">
         <f aca="false">SUM(B7:B9)-D11</f>
         <v>8</v>
       </c>
@@ -771,11 +799,11 @@
       <c r="G12" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="I12" s="28"/>
+      <c r="I12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
-      <c r="D13" s="27"/>
+      <c r="A13" s="27"/>
+      <c r="D13" s="25"/>
       <c r="F13" s="0" t="s">
         <v>16</v>
       </c>
@@ -783,11 +811,11 @@
         <f aca="false">(COLUMNS(Summary!$C$11:$D$12) - 1) * (ROWS(Summary!$C$11:$D$12) - 1)</f>
         <v>1</v>
       </c>
-      <c r="I13" s="28"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29"/>
-      <c r="D14" s="27"/>
+      <c r="A14" s="27"/>
+      <c r="D14" s="25"/>
       <c r="F14" s="0" t="s">
         <v>17</v>
       </c>
@@ -795,11 +823,11 @@
         <f aca="false">CHITEST(Summary!$C$11:$D$12, MMULT(MMULT(Summary!$C$11:$D$12,TRANSPOSE(IF(COLUMN(Summary!$C$11:$D$12),TRUE()))),MMULT(TRANSPOSE(IF(ROW(Summary!$C$11:$D$12),TRUE())),Summary!$C$11:$D$12)) / SUM(Summary!$C$11:$D$12))</f>
         <v>0.387614760141691</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29"/>
-      <c r="D15" s="27"/>
+      <c r="A15" s="27"/>
+      <c r="D15" s="25"/>
       <c r="F15" s="0" t="s">
         <v>18</v>
       </c>
@@ -807,47 +835,47 @@
         <f aca="false">CHIINV(Summary!$G$14, Summary!$G$13)</f>
         <v>0.746411483253589</v>
       </c>
-      <c r="I15" s="28"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="31" t="n">
+      <c r="G16" s="29" t="n">
         <f aca="false">CHIINV(Summary!$G$12, Summary!$G$13)</f>
         <v>3.84145882069413</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
-      <c r="D17" s="33"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="34" t="n">
+      <c r="B18" s="32" t="n">
         <f aca="false">AVERAGE(CC011!B$6:B$8)</f>
         <v>1</v>
       </c>
-      <c r="C18" s="34" t="n">
+      <c r="C18" s="32" t="n">
         <f aca="false">AVERAGE(CC011!C$6:C$8)</f>
         <v>1</v>
       </c>
-      <c r="D18" s="35" t="n">
+      <c r="D18" s="33" t="n">
         <f aca="false">AVERAGE(CC011!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="8" t="n">
@@ -858,13 +886,13 @@
         <f aca="false">AVERAGE(CC061!C$6:C$8)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="36" t="n">
+      <c r="D19" s="34" t="n">
         <f aca="false">AVERAGE(CC061!D$6:D$8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="8" t="n">
@@ -875,13 +903,13 @@
         <f aca="false">AVERAGE(CC017!C$6:C$8)</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="D20" s="36" t="n">
+      <c r="D20" s="34" t="n">
         <f aca="false">AVERAGE(CC017!D$6:D$8)</f>
         <v>0.666666666666667</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="8" t="n">
@@ -892,13 +920,13 @@
         <f aca="false">AVERAGE(CC092!C$6:C$8)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="D21" s="36" t="n">
+      <c r="D21" s="34" t="n">
         <f aca="false">AVERAGE(CC092!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="8" t="n">
@@ -909,13 +937,13 @@
         <f aca="false">AVERAGE(CC097!C$6:C$8)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="D22" s="36" t="n">
+      <c r="D22" s="34" t="n">
         <f aca="false">AVERAGE(CC097!D$6:D$8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="8" t="n">
@@ -926,13 +954,13 @@
         <f aca="false">AVERAGE(CC099!C$6:C$8)</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="D23" s="36" t="n">
+      <c r="D23" s="34" t="n">
         <f aca="false">AVERAGE(CC099!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="8" t="n">
@@ -943,13 +971,13 @@
         <f aca="false">AVERAGE(CC005!C$6:C$8)</f>
         <v>1</v>
       </c>
-      <c r="D24" s="36" t="n">
+      <c r="D24" s="34" t="n">
         <f aca="false">AVERAGE(CC005!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="8" t="n">
@@ -960,24 +988,24 @@
         <f aca="false">AVERAGE(CC026!C$6:C$8)</f>
         <v>1</v>
       </c>
-      <c r="D25" s="36" t="n">
+      <c r="D25" s="34" t="n">
         <f aca="false">AVERAGE(CC026!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="37" t="n">
+      <c r="B26" s="35" t="n">
         <f aca="false">AVERAGE(CC090!B$6:B$8)</f>
         <v>1</v>
       </c>
-      <c r="C26" s="37" t="n">
+      <c r="C26" s="35" t="n">
         <f aca="false">AVERAGE(CC090!C$6:C$8)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="38" t="n">
+      <c r="D26" s="36" t="n">
         <f aca="false">AVERAGE(CC090!D$6:D$8)</f>
         <v>0.333333333333333</v>
       </c>
@@ -1026,18 +1054,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1051,7 +1079,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1065,7 +1093,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1079,52 +1107,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1136,6 +1164,146 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>699</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>-0.172903583754429</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>-0.14673824601597</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.0171916528642093</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.0140603233337205</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.577348464967215</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.577348464967215</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">B6 / (B7 * SQRT(B4-1))</f>
+        <v>0.00112707263786992</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">C6 / (C7 * SQRT(C4-1))</f>
+        <v>0.000921784882129143</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">SQRT(B8^2 + C8^2)</f>
+        <v>0.00145601514413721</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">(B5-C5)/(B10)</f>
+        <v>-17.9705120814276</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">B4+C4-4</f>
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="40" t="n">
+        <f aca="false">TDIST(ABS(B11),B12,2)</f>
+        <v>4.15119739345655E-065</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1159,18 +1327,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1184,7 +1352,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1198,7 +1366,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1212,52 +1380,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1292,18 +1460,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1317,7 +1485,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1331,44 +1499,41 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="A8" s="37"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1400,18 +1565,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1425,7 +1590,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1439,7 +1604,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1453,52 +1618,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1533,18 +1698,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1558,7 +1723,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1572,7 +1737,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1586,52 +1751,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1666,18 +1831,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1691,7 +1856,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1705,7 +1870,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1719,52 +1884,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>0</v>
       </c>
@@ -1799,18 +1964,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1824,7 +1989,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1838,7 +2003,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1852,52 +2017,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1932,18 +2097,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1957,7 +2122,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1971,7 +2136,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1985,52 +2150,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -2065,18 +2230,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -2090,7 +2255,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -2104,7 +2269,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -2118,52 +2283,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="0" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="0" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="0" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated with F's changes. Still needs response document.
</commit_message>
<xml_diff>
--- a/python/event_results/results.xlsx
+++ b/python/event_results/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,6 @@
     <sheet name="CC005" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="CC026" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="CC090" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Obscuring Profile" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="29">
   <si>
     <t xml:space="preserve">test_x</t>
   </si>
@@ -117,39 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve">CC090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparison of Line Segments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stderr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x dev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slope dev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diff dev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t stat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p</t>
   </si>
 </sst>
 </file>
@@ -161,7 +127,7 @@
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,6 +157,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i val="true"/>
@@ -377,19 +349,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -405,31 +377,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,31 +465,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -532,17 +504,17 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,7 +574,7 @@
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">AVERAGE(CC011:CC090!B3:B3)</f>
-        <v>0.999828802214729</v>
+        <v>0.999828802214728</v>
       </c>
       <c r="C4" s="8" t="n">
         <f aca="false">AVERAGE(CC011:CC090!C3:C3)</f>
@@ -664,29 +636,29 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="n">
+      <c r="B7" s="15" t="n">
         <f aca="false">SUM(CC011:CC090!B6:B6)</f>
         <v>9</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="16" t="n">
         <f aca="false">SUM(CC011:CC090!C6:C6)</f>
         <v>5</v>
       </c>
-      <c r="D7" s="15" t="n">
+      <c r="D7" s="17" t="n">
         <f aca="false">SUM(CC011:CC090!D6:D6)</f>
         <v>6</v>
       </c>
@@ -720,15 +692,15 @@
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="14" t="n">
+      <c r="B8" s="15" t="n">
         <f aca="false">SUM(CC011:CC090!B7:B7)</f>
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="16" t="n">
         <f aca="false">SUM(CC011:CC090!C7:C7)</f>
         <v>6</v>
       </c>
-      <c r="D8" s="15" t="n">
+      <c r="D8" s="17" t="n">
         <f aca="false">SUM(CC011:CC090!D7:D7)</f>
         <v>5</v>
       </c>
@@ -738,58 +710,58 @@
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="14" t="n">
+      <c r="B9" s="15" t="n">
         <f aca="false">SUM(CC011:CC090!B8:B8)</f>
         <v>8</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="16" t="n">
         <f aca="false">SUM(CC011:CC090!C8:C8)</f>
         <v>4</v>
       </c>
-      <c r="D9" s="15" t="n">
+      <c r="D9" s="17" t="n">
         <f aca="false">SUM(CC011:CC090!D8:D8)</f>
         <v>7</v>
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+    <row r="10" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22" t="n">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24" t="n">
         <f aca="false">SUM(C7:C9)</f>
         <v>15</v>
       </c>
-      <c r="D11" s="22" t="n">
+      <c r="D11" s="24" t="n">
         <f aca="false">SUM(D7:D9)</f>
         <v>18</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25" t="n">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="n">
         <f aca="false">SUM(B7:B9)-C11</f>
         <v>11</v>
       </c>
-      <c r="D12" s="25" t="n">
+      <c r="D12" s="27" t="n">
         <f aca="false">SUM(B7:B9)-D11</f>
         <v>8</v>
       </c>
@@ -799,11 +771,11 @@
       <c r="G12" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="I12" s="26"/>
+      <c r="I12" s="28"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27"/>
-      <c r="D13" s="25"/>
+      <c r="A13" s="29"/>
+      <c r="D13" s="27"/>
       <c r="F13" s="0" t="s">
         <v>16</v>
       </c>
@@ -811,11 +783,11 @@
         <f aca="false">(COLUMNS(Summary!$C$11:$D$12) - 1) * (ROWS(Summary!$C$11:$D$12) - 1)</f>
         <v>1</v>
       </c>
-      <c r="I13" s="26"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27"/>
-      <c r="D14" s="25"/>
+      <c r="A14" s="29"/>
+      <c r="D14" s="27"/>
       <c r="F14" s="0" t="s">
         <v>17</v>
       </c>
@@ -823,11 +795,11 @@
         <f aca="false">CHITEST(Summary!$C$11:$D$12, MMULT(MMULT(Summary!$C$11:$D$12,TRANSPOSE(IF(COLUMN(Summary!$C$11:$D$12),TRUE()))),MMULT(TRANSPOSE(IF(ROW(Summary!$C$11:$D$12),TRUE())),Summary!$C$11:$D$12)) / SUM(Summary!$C$11:$D$12))</f>
         <v>0.387614760141691</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="29"/>
+      <c r="D15" s="27"/>
       <c r="F15" s="0" t="s">
         <v>18</v>
       </c>
@@ -835,47 +807,47 @@
         <f aca="false">CHIINV(Summary!$G$14, Summary!$G$13)</f>
         <v>0.746411483253589</v>
       </c>
-      <c r="I15" s="26"/>
+      <c r="I15" s="28"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="29" t="n">
+      <c r="G16" s="31" t="n">
         <f aca="false">CHIINV(Summary!$G$12, Summary!$G$13)</f>
         <v>3.84145882069413</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="30"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
-      <c r="D17" s="31"/>
+      <c r="D17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="32" t="n">
+      <c r="B18" s="34" t="n">
         <f aca="false">AVERAGE(CC011!B$6:B$8)</f>
         <v>1</v>
       </c>
-      <c r="C18" s="32" t="n">
+      <c r="C18" s="34" t="n">
         <f aca="false">AVERAGE(CC011!C$6:C$8)</f>
         <v>1</v>
       </c>
-      <c r="D18" s="33" t="n">
+      <c r="D18" s="35" t="n">
         <f aca="false">AVERAGE(CC011!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="8" t="n">
@@ -886,13 +858,13 @@
         <f aca="false">AVERAGE(CC061!C$6:C$8)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="34" t="n">
+      <c r="D19" s="36" t="n">
         <f aca="false">AVERAGE(CC061!D$6:D$8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="8" t="n">
@@ -903,13 +875,13 @@
         <f aca="false">AVERAGE(CC017!C$6:C$8)</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="D20" s="34" t="n">
+      <c r="D20" s="36" t="n">
         <f aca="false">AVERAGE(CC017!D$6:D$8)</f>
         <v>0.666666666666667</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="8" t="n">
@@ -920,13 +892,13 @@
         <f aca="false">AVERAGE(CC092!C$6:C$8)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="D21" s="34" t="n">
+      <c r="D21" s="36" t="n">
         <f aca="false">AVERAGE(CC092!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="8" t="n">
@@ -937,13 +909,13 @@
         <f aca="false">AVERAGE(CC097!C$6:C$8)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="D22" s="34" t="n">
+      <c r="D22" s="36" t="n">
         <f aca="false">AVERAGE(CC097!D$6:D$8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="8" t="n">
@@ -954,13 +926,13 @@
         <f aca="false">AVERAGE(CC099!C$6:C$8)</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="D23" s="34" t="n">
+      <c r="D23" s="36" t="n">
         <f aca="false">AVERAGE(CC099!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="8" t="n">
@@ -971,13 +943,13 @@
         <f aca="false">AVERAGE(CC005!C$6:C$8)</f>
         <v>1</v>
       </c>
-      <c r="D24" s="34" t="n">
+      <c r="D24" s="36" t="n">
         <f aca="false">AVERAGE(CC005!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="8" t="n">
@@ -988,24 +960,24 @@
         <f aca="false">AVERAGE(CC026!C$6:C$8)</f>
         <v>1</v>
       </c>
-      <c r="D25" s="34" t="n">
+      <c r="D25" s="36" t="n">
         <f aca="false">AVERAGE(CC026!D$6:D$8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="35" t="n">
+      <c r="B26" s="37" t="n">
         <f aca="false">AVERAGE(CC090!B$6:B$8)</f>
         <v>1</v>
       </c>
-      <c r="C26" s="35" t="n">
+      <c r="C26" s="37" t="n">
         <f aca="false">AVERAGE(CC090!C$6:C$8)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="36" t="n">
+      <c r="D26" s="38" t="n">
         <f aca="false">AVERAGE(CC090!D$6:D$8)</f>
         <v>0.333333333333333</v>
       </c>
@@ -1054,18 +1026,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1079,7 +1051,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1093,7 +1065,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1107,52 +1079,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1164,146 +1136,6 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>699</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>-0.172903583754429</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>-0.14673824601597</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0.0171916528642093</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.0140603233337205</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0.577348464967215</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0.577348464967215</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <f aca="false">B6 / (B7 * SQRT(B4-1))</f>
-        <v>0.00112707263786992</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <f aca="false">C6 / (C7 * SQRT(C4-1))</f>
-        <v>0.000921784882129143</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <f aca="false">SQRT(B8^2 + C8^2)</f>
-        <v>0.00145601514413721</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <f aca="false">(B5-C5)/(B10)</f>
-        <v>-17.9705120814276</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <f aca="false">B4+C4-4</f>
-        <v>1394</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="40" t="n">
-        <f aca="false">TDIST(ABS(B11),B12,2)</f>
-        <v>4.15119739345655E-065</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1327,18 +1159,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1352,7 +1184,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1366,7 +1198,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1380,52 +1212,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1460,18 +1292,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1485,7 +1317,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1499,41 +1331,44 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1565,18 +1400,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1590,7 +1425,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1604,7 +1439,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1618,52 +1453,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1698,18 +1533,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1723,7 +1558,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1737,7 +1572,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1751,52 +1586,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -1831,18 +1666,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1856,7 +1691,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1870,7 +1705,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1884,52 +1719,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>0</v>
       </c>
@@ -1964,18 +1799,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1989,7 +1824,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -2003,7 +1838,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -2017,52 +1852,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>0</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -2097,18 +1932,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -2122,7 +1957,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -2136,7 +1971,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -2150,52 +1985,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>
@@ -2230,18 +2065,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -2255,7 +2090,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -2269,7 +2104,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -2283,52 +2118,52 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="40" t="n">
         <f aca="false">B2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="40" t="n">
         <f aca="false">C2&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="40" t="n">
         <f aca="false">D2&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="40" t="n">
         <f aca="false">B3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="40" t="n">
         <f aca="false">C3&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="40" t="n">
         <f aca="false">D3&gt;=0.5</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="40" t="n">
         <f aca="false">B4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="40" t="n">
         <f aca="false">C4&gt;=0.5</f>
         <v>1</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="40" t="n">
         <f aca="false">D4&gt;=0.5</f>
         <v>1</v>
       </c>

</xml_diff>